<commit_message>
Script de criacao do BD
</commit_message>
<xml_diff>
--- a/Documentos/Banco de dados/DER.xlsx
+++ b/Documentos/Banco de dados/DER.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>Modelo Relacional</t>
   </si>
@@ -203,9 +203,6 @@
     <t>char(1)</t>
   </si>
   <si>
-    <t>id_nr_subitem</t>
-  </si>
-  <si>
     <t>subitem</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t>id_processo</t>
   </si>
   <si>
-    <t>local</t>
-  </si>
-  <si>
     <t>medida_corretiva</t>
   </si>
   <si>
@@ -249,6 +243,33 @@
   </si>
   <si>
     <t>multa</t>
+  </si>
+  <si>
+    <t>localizacao</t>
+  </si>
+  <si>
+    <t>id_relator</t>
+  </si>
+  <si>
+    <t>id_resp_correcao</t>
+  </si>
+  <si>
+    <t>processo_nr</t>
+  </si>
+  <si>
+    <t>maquina | id_maquina</t>
+  </si>
+  <si>
+    <t>Relator do processo</t>
+  </si>
+  <si>
+    <t>Responsável pela correção</t>
+  </si>
+  <si>
+    <t>maquina do processo</t>
+  </si>
+  <si>
+    <t>id_nr_item</t>
   </si>
 </sst>
 </file>
@@ -319,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -379,34 +400,42 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -417,45 +446,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="6"/>
@@ -812,1051 +820,1166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H88"/>
+  <dimension ref="B2:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85:H88"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="11"/>
-    <col min="2" max="2" width="17.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.75" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.875" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="11"/>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="17.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="16"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="16"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+      <c r="C16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
+      <c r="C17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
+      <c r="C18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="C19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="C20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="C21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="C22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="C23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16" t="s">
+      <c r="D25" s="9"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="14"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="H29" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="16"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="C31" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
+      <c r="C32" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="C33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="C34" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+      <c r="C35" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
+      <c r="C36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
+      <c r="C37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="C38" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="C39" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
+      <c r="C40" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="16"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16" t="s">
+      <c r="D41" s="9"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16" t="s">
+      <c r="D42" s="9"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="10"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="14"/>
     </row>
     <row r="46" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="G46" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H46" s="15" t="s">
+      <c r="H46" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6" t="s">
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H47" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
+      <c r="C48" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
+      <c r="C50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="10"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="14"/>
     </row>
     <row r="54" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="G54" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H54" s="15" t="s">
+      <c r="H54" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="13"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="16"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="9"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="10"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="14"/>
     </row>
     <row r="62" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G62" s="5" t="s">
+      <c r="G62" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H62" s="15" t="s">
+      <c r="H62" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D63" s="13"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
-      <c r="H63" s="16"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="9"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
+      <c r="C64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C65" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
+      <c r="C65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C66" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
+      <c r="C66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C67" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B70" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" s="9"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B73" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="14"/>
+    </row>
+    <row r="74" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H74" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B75" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" s="6"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="9"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B76" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B77" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B80" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D69" s="16"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" s="16" t="s">
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="14"/>
+    </row>
+    <row r="81" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B82" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D82" s="6"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="9"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B83" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B84" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B86" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B87" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B88" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B89" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="16"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="8" t="s">
+      <c r="D89" s="9"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B90" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D90" s="9"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B91" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="10"/>
-    </row>
-    <row r="74" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B74" s="5" t="s">
+      <c r="C91" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" s="9"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H91" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B94" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="14"/>
+    </row>
+    <row r="95" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C95" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D95" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E95" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F95" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G74" s="5" t="s">
+      <c r="G95" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H74" s="15" t="s">
+      <c r="H95" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B75" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D75" s="13"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="16"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B76" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76" s="16"/>
-      <c r="E76" s="16"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="16"/>
-      <c r="H76" s="16"/>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B77" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C77" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="16"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="16"/>
-      <c r="H77" s="16"/>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B80" s="8" t="s">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B96" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="10"/>
-    </row>
-    <row r="81" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B81" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H81" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B82" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="13"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
-      <c r="H82" s="16"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B83" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C83" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D83" s="16"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="16"/>
-      <c r="H83" s="16"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B84" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C84" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C85" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D85" s="16"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B86" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C86" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D86" s="16"/>
-      <c r="E86" s="16"/>
-      <c r="F86" s="16"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="16"/>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B87" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C87" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D87" s="16"/>
-      <c r="E87" s="16"/>
-      <c r="F87" s="16"/>
-      <c r="G87" s="16"/>
-      <c r="H87" s="16"/>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B88" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C88" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D88" s="16"/>
-      <c r="E88" s="16"/>
-      <c r="F88" s="16"/>
-      <c r="G88" s="16"/>
-      <c r="H88" s="16"/>
+      <c r="C96" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="9"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B97" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="B94:H94"/>
     <mergeCell ref="B73:H73"/>
     <mergeCell ref="B80:H80"/>
     <mergeCell ref="B7:H7"/>
@@ -1865,46 +1988,48 @@
     <mergeCell ref="B45:H45"/>
     <mergeCell ref="B53:H53"/>
     <mergeCell ref="B61:H61"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
   </mergeCells>
   <conditionalFormatting sqref="E10:F10 D9">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:F15">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:F15">
+  <conditionalFormatting sqref="D30:F30">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:F30">
+  <conditionalFormatting sqref="D47:F47">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47:F47">
+  <conditionalFormatting sqref="D55:F55">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55:F55">
+  <conditionalFormatting sqref="D63:F63">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63:F63">
+  <conditionalFormatting sqref="D75:F75">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D75:F75">
+  <conditionalFormatting sqref="D82:F82">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D82:F82">
+  <conditionalFormatting sqref="D96:F96">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>